<commit_message>
removed spaces and quotation marks from files
</commit_message>
<xml_diff>
--- a/VO2_data/subject_1232.xlsx
+++ b/VO2_data/subject_1232.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc.sharepoint.com/sites/KNES606/Shared Documents/General/Subjects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Holash\Documents\Knes381\VO2_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15AA80A1-B6B0-4C72-9A2D-0E2DE57209FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342EE50A-1FC3-473E-B3A2-508DC3B72EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="1464" windowWidth="34812" windowHeight="23784" xr2:uid="{50C3FD67-14AF-4C51-A6CF-164A5BDC9CC9}"/>
+    <workbookView xWindow="18396" yWindow="2052" windowWidth="22080" windowHeight="23268" xr2:uid="{50C3FD67-14AF-4C51-A6CF-164A5BDC9CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,109 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
-  <si>
-    <t xml:space="preserve">TIME </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "VO2   "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "VO2/kg  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "METS "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "VCO2  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "VE     "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "RER  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "RR  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Vt    "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "FEO2  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "FECO2 "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "HR  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "VE/   "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "PetCO2 "</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "STPD  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "STPD    "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "     "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "BTPS   "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "    "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "BTPS  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "      "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "       "</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "L/min "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "ml/kg/m "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "L/min  "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "BPM "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "L     "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "%     "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "bpm "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "BT/ST "</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "mmHg   "</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>W</t>
   </si>
@@ -147,6 +45,87 @@
   </si>
   <si>
     <t>----------</t>
+  </si>
+  <si>
+    <t>METS</t>
+  </si>
+  <si>
+    <t>FECO2</t>
+  </si>
+  <si>
+    <t>PetCO2</t>
+  </si>
+  <si>
+    <t>L/min</t>
+  </si>
+  <si>
+    <t>ml/kg/m</t>
+  </si>
+  <si>
+    <t>BPM</t>
+  </si>
+  <si>
+    <t>bpm</t>
+  </si>
+  <si>
+    <t>BT/ST</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>VO2</t>
+  </si>
+  <si>
+    <t>VO2/kg</t>
+  </si>
+  <si>
+    <t>VCO2</t>
+  </si>
+  <si>
+    <t>VE</t>
+  </si>
+  <si>
+    <t>RER</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>Vt</t>
+  </si>
+  <si>
+    <t>FEO2</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>STPD</t>
+  </si>
+  <si>
+    <t>BTPS</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>VE/VO2</t>
+  </si>
+  <si>
+    <t>VE/VCO2</t>
   </si>
 </sst>
 </file>
@@ -501,105 +480,75 @@
   <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Q58"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -608,57 +557,51 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" t="s">
-        <v>33</v>
-      </c>
       <c r="P3" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -3394,6 +3337,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d313e902-e84c-44a8-9828-797d5a3290d9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7b80b8b-1f02-4dc1-97da-babab5d0e31f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001BFAF3A11B2F1D4C871B4AAFA789A753" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c0be2542df2ec9155b2312bbc42eacc5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e7b80b8b-1f02-4dc1-97da-babab5d0e31f" xmlns:ns3="d313e902-e84c-44a8-9828-797d5a3290d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73d1dbb1edd46924ab85676eaa35fa73" ns2:_="" ns3:_="">
     <xsd:import namespace="e7b80b8b-1f02-4dc1-97da-babab5d0e31f"/>
@@ -3636,34 +3599,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d313e902-e84c-44a8-9828-797d5a3290d9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7b80b8b-1f02-4dc1-97da-babab5d0e31f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D6FDD75-CE78-495D-A703-1514760377DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20C46174-B2F9-49A2-8E1E-D6B381DBB365}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d313e902-e84c-44a8-9828-797d5a3290d9"/>
+    <ds:schemaRef ds:uri="e7b80b8b-1f02-4dc1-97da-babab5d0e31f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCF19870-61AA-4C60-BCDE-A0FF90E06B5F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCF19870-61AA-4C60-BCDE-A0FF90E06B5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20C46174-B2F9-49A2-8E1E-D6B381DBB365}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D6FDD75-CE78-495D-A703-1514760377DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e7b80b8b-1f02-4dc1-97da-babab5d0e31f"/>
+    <ds:schemaRef ds:uri="d313e902-e84c-44a8-9828-797d5a3290d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>